<commit_message>
I cannot remember what I did here... oops!
</commit_message>
<xml_diff>
--- a/density_data/Landcover.xlsx
+++ b/density_data/Landcover.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljohnso8\Desktop\lidar\RECLASSIFY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/density_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9819C988-4254-184C-ACCE-EC5BE4DFF2A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23130" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="320" yWindow="2280" windowWidth="26960" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="drainbasin" sheetId="1" r:id="rId1"/>
     <sheet name="huc12" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>site_id</t>
   </si>
@@ -157,12 +166,15 @@
   </si>
   <si>
     <t>Tdvlp</t>
+  </si>
+  <si>
+    <t>Rprc_TH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,21 +486,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +553,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -602,7 +614,7 @@
         <v>23.515349813340876</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -663,7 +675,7 @@
         <v>23.293223338136894</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -724,7 +736,7 @@
         <v>23.277941161254976</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -785,7 +797,7 @@
         <v>23.237906024787016</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -846,7 +858,7 @@
         <v>24.115271346302684</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -907,7 +919,7 @@
         <v>23.924137432596083</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -968,7 +980,7 @@
         <v>22.619144687908932</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1041,7 @@
         <v>22.487068476269233</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>22.148457977188325</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1163,7 @@
         <v>23.56002820032759</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1224,7 @@
         <v>20.426526997234649</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1273,7 +1285,7 @@
         <v>16.380902360096911</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>20.196395296457574</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1395,7 +1407,7 @@
         <v>16.302463422798969</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1456,7 +1468,7 @@
         <v>20.116251191173088</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1529,7 @@
         <v>20.182547476196486</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1578,7 +1590,7 @@
         <v>24.115271346302684</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1645,22 +1657,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1715,8 +1727,11 @@
       <c r="R1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>171003021305</v>
       </c>
@@ -1779,8 +1794,12 @@
         <f xml:space="preserve"> G2/K2 * 100</f>
         <v>19.112783889853954</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2">
+        <f>G2/(G2+H2) *100</f>
+        <v>46.756905642559218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>171003021102</v>
       </c>
@@ -1843,8 +1862,12 @@
         <f t="shared" ref="R3:R9" si="7" xml:space="preserve"> G3/K3 * 100</f>
         <v>38.688573282162317</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <f t="shared" ref="S3:S9" si="8">G3/(G3+H3) *100</f>
+        <v>49.500960076806145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>171003020508</v>
       </c>
@@ -1907,8 +1930,12 @@
         <f t="shared" si="7"/>
         <v>22.111588846144176</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <f t="shared" si="8"/>
+        <v>29.538812938765911</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>171003020506</v>
       </c>
@@ -1971,8 +1998,12 @@
         <f t="shared" si="7"/>
         <v>29.489491794261742</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5">
+        <f t="shared" si="8"/>
+        <v>32.090757238307347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>171003020502</v>
       </c>
@@ -2035,8 +2066,12 @@
         <f t="shared" si="7"/>
         <v>45.387215337162701</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6">
+        <f t="shared" si="8"/>
+        <v>47.999843737792013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>171003020306</v>
       </c>
@@ -2099,8 +2134,12 @@
         <f t="shared" si="7"/>
         <v>21.066384485811774</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7">
+        <f t="shared" si="8"/>
+        <v>21.450875186911777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>171003020903</v>
       </c>
@@ -2163,8 +2202,12 @@
         <f t="shared" si="7"/>
         <v>29.747091066448693</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8">
+        <f t="shared" si="8"/>
+        <v>31.204228619847886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>171003020902</v>
       </c>
@@ -2226,6 +2269,10 @@
       <c r="R9">
         <f t="shared" si="7"/>
         <v>47.343896787123441</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="8"/>
+        <v>49.3336813939829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>